<commit_message>
Manufacturer and Brands 20 scripts complete
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ManufacturerBrandModuleTest.xlsx
+++ b/resources/ExcelsheetData/ManufacturerBrandModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="21" activeTab="28"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TC_MB_001" sheetId="21" r:id="rId1"/>
@@ -12,37 +12,40 @@
     <sheet name="TC_MB_002" sheetId="3" r:id="rId3"/>
     <sheet name="TC_MB_002_1" sheetId="5" r:id="rId4"/>
     <sheet name="TC_MB_004" sheetId="4" r:id="rId5"/>
-    <sheet name="TC_MB_006" sheetId="22" r:id="rId6"/>
-    <sheet name="TC_MB_010" sheetId="23" r:id="rId7"/>
-    <sheet name="TC_MB_011" sheetId="24" r:id="rId8"/>
-    <sheet name="TC_MB_012" sheetId="25" r:id="rId9"/>
-    <sheet name="TC_MB_013" sheetId="26" r:id="rId10"/>
-    <sheet name="TC_MB_014" sheetId="27" r:id="rId11"/>
-    <sheet name="TC_MB_019" sheetId="28" r:id="rId12"/>
-    <sheet name="TC_MB_023" sheetId="6" r:id="rId13"/>
-    <sheet name="TC_MB_026_1" sheetId="7" r:id="rId14"/>
-    <sheet name="TC_MB_030" sheetId="8" r:id="rId15"/>
-    <sheet name="TC_MB_032" sheetId="9" r:id="rId16"/>
-    <sheet name="TC_MB_033" sheetId="10" r:id="rId17"/>
-    <sheet name="TC_MB_035" sheetId="11" r:id="rId18"/>
-    <sheet name="TC_MB_036" sheetId="12" r:id="rId19"/>
-    <sheet name="TC_MB_039" sheetId="13" r:id="rId20"/>
-    <sheet name="TC_MB_039_1" sheetId="14" r:id="rId21"/>
-    <sheet name="TC_MB_041" sheetId="17" r:id="rId22"/>
-    <sheet name="TC_MB_042" sheetId="18" r:id="rId23"/>
-    <sheet name="TC_MB_043" sheetId="19" r:id="rId24"/>
-    <sheet name="TC_MB_043_1" sheetId="20" r:id="rId25"/>
-    <sheet name="verifyCharLimitManuName" sheetId="29" r:id="rId26"/>
-    <sheet name="verifyCharLimitManuCode" sheetId="30" r:id="rId27"/>
-    <sheet name="TC_MB_047" sheetId="15" r:id="rId28"/>
-    <sheet name="TC_MB_048" sheetId="16" r:id="rId29"/>
+    <sheet name="TC_MB_009" sheetId="32" r:id="rId6"/>
+    <sheet name="TC_MB_006" sheetId="22" r:id="rId7"/>
+    <sheet name="TC_MB_010" sheetId="23" r:id="rId8"/>
+    <sheet name="TC_MB_011" sheetId="24" r:id="rId9"/>
+    <sheet name="TC_MB_012" sheetId="25" r:id="rId10"/>
+    <sheet name="TC_MB_013" sheetId="26" r:id="rId11"/>
+    <sheet name="TC_MB_016" sheetId="33" r:id="rId12"/>
+    <sheet name="TC_MB_014" sheetId="27" r:id="rId13"/>
+    <sheet name="TC_MB_019" sheetId="28" r:id="rId14"/>
+    <sheet name="TC_MB_023" sheetId="6" r:id="rId15"/>
+    <sheet name="TC_MB_026_1" sheetId="7" r:id="rId16"/>
+    <sheet name="TC_MB_030" sheetId="8" r:id="rId17"/>
+    <sheet name="TC_MB_032" sheetId="9" r:id="rId18"/>
+    <sheet name="TC_MB_033" sheetId="10" r:id="rId19"/>
+    <sheet name="TC_MB_035" sheetId="11" r:id="rId20"/>
+    <sheet name="TC_MB_036" sheetId="12" r:id="rId21"/>
+    <sheet name="TC_MB_039" sheetId="13" r:id="rId22"/>
+    <sheet name="TC_MB_039_1" sheetId="14" r:id="rId23"/>
+    <sheet name="TC_MB_041" sheetId="17" r:id="rId24"/>
+    <sheet name="TC_MB_042" sheetId="18" r:id="rId25"/>
+    <sheet name="TC_MB_043" sheetId="19" r:id="rId26"/>
+    <sheet name="TC_MB_043_1" sheetId="20" r:id="rId27"/>
+    <sheet name="verifyCharLimitManuName" sheetId="29" r:id="rId28"/>
+    <sheet name="verifyCharLimitManuCode" sheetId="30" r:id="rId29"/>
+    <sheet name="TC_MB_047" sheetId="15" r:id="rId30"/>
+    <sheet name="TC_MB_048" sheetId="16" r:id="rId31"/>
+    <sheet name="createManufacturers" sheetId="31" r:id="rId32"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="96">
   <si>
     <t>Manufacturers Name</t>
   </si>
@@ -285,6 +288,51 @@
   </si>
   <si>
     <t>automationUse</t>
+  </si>
+  <si>
+    <t>testCaseID</t>
+  </si>
+  <si>
+    <t>manufacturersName</t>
+  </si>
+  <si>
+    <t>manufacturersCode</t>
+  </si>
+  <si>
+    <t>manufacturerActiveStatus</t>
+  </si>
+  <si>
+    <t>saveMessage</t>
+  </si>
+  <si>
+    <t>TC_M-Brands_1</t>
+  </si>
+  <si>
+    <t>cimmAdmin</t>
+  </si>
+  <si>
+    <t>adminCimm86$$</t>
+  </si>
+  <si>
+    <t>ATManu</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>Search Keyword</t>
+  </si>
+  <si>
+    <t>Invalidkeyword111</t>
+  </si>
+  <si>
+    <t>fieldnames</t>
+  </si>
+  <si>
+    <t>Manufacturer Logo,Manufacturer Id,Status</t>
   </si>
 </sst>
 </file>
@@ -676,14 +724,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,7 +766,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,6 +845,95 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -836,7 +973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -885,7 +1022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -967,7 +1104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1016,7 +1153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1072,7 +1209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1114,104 +1251,6 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1843,6 +1882,104 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1897,7 +2034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1946,7 +2083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1995,7 +2132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2044,12 +2181,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,7 +2286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2226,7 +2363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2267,7 +2404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2308,110 +2445,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,12 +2515,181 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,6 +2817,95 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2648,7 +2945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2687,86 +2984,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>